<commit_message>
Added some information according to the updated textfile
</commit_message>
<xml_diff>
--- a/projekt-dokumentation/Slutrapporten/ekvivalensklasserTestmatris.xlsx
+++ b/projekt-dokumentation/Slutrapporten/ekvivalensklasserTestmatris.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="17">
   <si>
     <t>subtractChips(int bet)</t>
   </si>
@@ -57,7 +57,16 @@
     <t>players *</t>
   </si>
   <si>
-    <t>// Vi kommer behöva förklara att inga Players är en valid ekvivalensklass också</t>
+    <t>// Vi kommer behöva förklara att inga parametrar är en valid ekvivalensklass också</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>valid</t>
+  </si>
+  <si>
+    <t>players = null</t>
   </si>
 </sst>
 </file>
@@ -389,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -402,46 +411,46 @@
     <col min="3" max="3" width="14.85546875" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
     <col min="5" max="5" width="27.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="6" max="7" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8">
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3">
+    <row r="4" spans="1:8">
+      <c r="A4">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4">
-        <v>2</v>
-      </c>
       <c r="C4" t="s">
         <v>2</v>
       </c>
@@ -449,122 +458,164 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6">
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7">
         <v>4</v>
       </c>
-      <c r="D6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
+    <row r="10" spans="1:8">
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
         <v>1</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C11" t="s">
         <v>7</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D11" t="s">
         <v>6</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E11" t="s">
         <v>5</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F11" t="s">
         <v>12</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
-      <c r="A10">
+    <row r="12" spans="1:8">
+      <c r="A12">
         <v>1</v>
       </c>
-      <c r="C10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" t="s">
-        <v>2</v>
-      </c>
-      <c r="G10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12">
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14">
         <v>3</v>
       </c>
-      <c r="G12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13">
+      <c r="H14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15">
         <v>4</v>
       </c>
-      <c r="B13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" t="s">
-        <v>2</v>
-      </c>
-      <c r="G13" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14">
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16">
         <v>5</v>
       </c>
-      <c r="C14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" t="s">
-        <v>2</v>
-      </c>
-      <c r="G14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" t="s">
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ekvivalens: Updated testcases. Gave each testcase a name ekvivalensklasserTestmatris: took away non-used testcase GameTest: Updated parameters to better fit the dokument PlayerTest: Added missing testcases
</commit_message>
<xml_diff>
--- a/projekt-dokumentation/Slutrapporten/ekvivalensklasserTestmatris.xlsx
+++ b/projekt-dokumentation/Slutrapporten/ekvivalensklasserTestmatris.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="17">
   <si>
     <t>subtractChips(int bet)</t>
   </si>
@@ -398,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -574,7 +574,10 @@
       <c r="A14">
         <v>3</v>
       </c>
-      <c r="H14" t="s">
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
         <v>2</v>
       </c>
     </row>
@@ -582,10 +585,10 @@
       <c r="A15">
         <v>4</v>
       </c>
-      <c r="B15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
         <v>2</v>
       </c>
     </row>
@@ -596,26 +599,15 @@
       <c r="C16" t="s">
         <v>2</v>
       </c>
-      <c r="D16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17">
-        <v>6</v>
-      </c>
-      <c r="C17" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" t="s">
-        <v>2</v>
-      </c>
-      <c r="G17" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" t="s">
+      <c r="E16" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>